<commit_message>
with excel df - 2048
</commit_message>
<xml_diff>
--- a/DTS_out offset/2.xlsx
+++ b/DTS_out offset/2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SinhaAd\Desktop\ADC\4_o\adc_4\DTS_out offset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adity\Desktop\adc_4\DTS_out offset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF52369E-29E6-456E-BCF7-6FEE32DDE072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF647C-0465-443D-B9E3-D18DC5EE96B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1F390A24-7B0C-4EDA-82A8-80FD5132F336}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1F390A24-7B0C-4EDA-82A8-80FD5132F336}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DF = 512" sheetId="1" r:id="rId1"/>
+    <sheet name="DF = 2048" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t xml:space="preserve">vs </t>
   </si>
@@ -63,13 +64,31 @@
   </si>
   <si>
     <t>Diff error wrt vs=0</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF </t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>vs</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Error mar wrt to vs = 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,8 +96,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +115,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -104,9 +137,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,18 +479,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3D7CDA-38CE-4AA1-BAFC-47F6DC3D251D}">
-  <dimension ref="B1:R10"/>
+  <dimension ref="B1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -528,7 +566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -566,7 +604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>5.1199999999999998E-4</v>
       </c>
@@ -604,7 +642,7 @@
         <v>34335</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1.024E-3</v>
       </c>
@@ -642,7 +680,7 @@
         <v>34340</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.536E-3</v>
       </c>
@@ -680,7 +718,7 @@
         <v>34331</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>8</v>
       </c>
@@ -705,7 +743,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F9">
         <f t="shared" ref="F9:F10" si="0">($F5-$C5)</f>
         <v>1</v>
@@ -727,13 +765,13 @@
         <v>494</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F10">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I9:I10" si="2">($I6-$C6)</f>
+        <f t="shared" ref="I10" si="2">($I6-$C6)</f>
         <v>-2</v>
       </c>
       <c r="L10">
@@ -749,7 +787,356 @@
         <v>484</v>
       </c>
     </row>
+    <row r="13" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>512</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D588564-6C70-42EA-825C-9D6B8A655B2A}">
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2.0479999999999999E-3</v>
+      </c>
+      <c r="D5">
+        <v>541498</v>
+      </c>
+      <c r="F5">
+        <v>2.0479999999999999E-3</v>
+      </c>
+      <c r="G5">
+        <v>541514</v>
+      </c>
+      <c r="I5">
+        <v>2.0479999999999999E-3</v>
+      </c>
+      <c r="J5">
+        <v>541571</v>
+      </c>
+      <c r="L5">
+        <v>2.0479999999999999E-3</v>
+      </c>
+      <c r="M5">
+        <v>542293</v>
+      </c>
+      <c r="O5">
+        <v>2.0479999999999999E-3</v>
+      </c>
+      <c r="P5">
+        <v>545411</v>
+      </c>
+      <c r="R5">
+        <v>2.0479999999999999E-3</v>
+      </c>
+      <c r="S5">
+        <v>549323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4.0959999999999998E-3</v>
+      </c>
+      <c r="D6">
+        <v>541492</v>
+      </c>
+      <c r="F6">
+        <v>4.0959999999999998E-3</v>
+      </c>
+      <c r="G6">
+        <v>541498</v>
+      </c>
+      <c r="I6">
+        <v>4.0959999999999998E-3</v>
+      </c>
+      <c r="J6">
+        <v>541579</v>
+      </c>
+      <c r="L6">
+        <v>4.0959999999999998E-3</v>
+      </c>
+      <c r="M6">
+        <v>542284</v>
+      </c>
+      <c r="O6">
+        <v>4.0959999999999998E-3</v>
+      </c>
+      <c r="P6">
+        <v>545417</v>
+      </c>
+      <c r="R6">
+        <v>4.0959999999999998E-3</v>
+      </c>
+      <c r="S6">
+        <v>549321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>6.1440000000000002E-3</v>
+      </c>
+      <c r="D7">
+        <v>541508</v>
+      </c>
+      <c r="F7">
+        <v>6.1440000000000002E-3</v>
+      </c>
+      <c r="G7">
+        <v>541512</v>
+      </c>
+      <c r="I7">
+        <v>6.1440000000000002E-3</v>
+      </c>
+      <c r="J7">
+        <v>541584</v>
+      </c>
+      <c r="L7">
+        <v>6.1440000000000002E-3</v>
+      </c>
+      <c r="M7">
+        <v>542281</v>
+      </c>
+      <c r="O7">
+        <v>6.1440000000000002E-3</v>
+      </c>
+      <c r="P7">
+        <v>545409</v>
+      </c>
+      <c r="R7">
+        <v>6.1440000000000002E-3</v>
+      </c>
+      <c r="S7">
+        <v>549325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="G9">
+        <f>$G4 - $D4</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>$J4 - $D4</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>$M4 - $D4</f>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f>$P4 - $D4</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f>$S4 - $D4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>$G5 - $D5</f>
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:J12" si="0">$J5 - $D5</f>
+        <v>73</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:M12" si="1">$M5 - $D5</f>
+        <v>795</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10:P12" si="2">$P5 - $D5</f>
+        <v>3913</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ref="S10:S12" si="3">$S5 - $D5</f>
+        <v>7825</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" ref="G11:G12" si="4">$G6 - $D6</f>
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>792</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>3925</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>7829</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>773</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>3901</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>7817</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>